<commit_message>
primeira versão completa e funcional
</commit_message>
<xml_diff>
--- a/datasets/pfp.xlsx
+++ b/datasets/pfp.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="pfp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
   <si>
     <t>NLQ</t>
   </si>
@@ -223,6 +223,51 @@
   </si>
   <si>
     <t>SELECT field, state, AVG(oil_production) as avg_oil_production FROM (SELECT field, state, SUM(oil_production) as oil_production FROM NLIDB_RESULT_SET GROUP BY field, state, year) GROUP BY field, state ORDER BY field, state</t>
+  </si>
+  <si>
+    <t>insert</t>
+  </si>
+  <si>
+    <t>Which field produces the most oil per month?</t>
+  </si>
+  <si>
+    <t>Which field produces the oil month?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT field, oil_production, year, month FROM ANP </t>
+  </si>
+  <si>
+    <t>SELECT year, month, field, max(oil_production) as max_oil_production FROM NLIDB_RESULT_SET GROUP BY year, month, field ORDER BY year, month, field</t>
+  </si>
+  <si>
+    <t>Which basin has the highest yearly oil production?</t>
+  </si>
+  <si>
+    <t>Which basin has the year oil production?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT basin, year, oil_production FROM ANP </t>
+  </si>
+  <si>
+    <t>SELECT basin, max(oil_production) as max_oil_production FROM (SELECT basin, SUM(oil_production) as oil_production FROM NLIDB_RESULT_SET GROUP BY basin, year) GROUP BY basin ORDER BY basin</t>
+  </si>
+  <si>
+    <t>Which federated state has the lowest gas production?</t>
+  </si>
+  <si>
+    <t>Which federated state has the gas production?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT state, gas_production FROM ANP </t>
+  </si>
+  <si>
+    <t>SELECT state, min(gas_production) as min_gas_production FROM NLIDB_RESULT_SET GROUP BY state ORDER BY state</t>
+  </si>
+  <si>
+    <t>Which state of the federation has the lowest gas production?</t>
+  </si>
+  <si>
+    <t>Which state of the federation has the gas production?</t>
   </si>
 </sst>
 </file>
@@ -767,13 +812,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D18" totalsRowShown="0">
-  <autoFilter ref="A1:D18"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:E22" totalsRowShown="0">
+  <autoFilter ref="A1:E22"/>
+  <tableColumns count="5">
     <tableColumn id="4" name="NLQ"/>
     <tableColumn id="1" name="NLQ preproccessed by GLAMORISE"/>
     <tableColumn id="2" name="NLIDB SQL"/>
     <tableColumn id="3" name="GLAMORISE SQL"/>
+    <tableColumn id="5" name="insert">
+      <calculatedColumnFormula>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1042,21 +1090,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="91.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="192.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="90.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="192.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="206.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1069,8 +1118,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1083,8 +1135,12 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the production of oil in state of Rio de Janeiro?', 'SELECT oil_production FROM ANP WHERE lower(state) = ''rio de janeiro''');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1097,8 +1153,12 @@
       <c r="D3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month production of oil in state of Rio de Janeiro?', 'SELECT year, month, oil_production FROM ANP WHERE lower(state) = ''rio de janeiro''');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1111,8 +1171,12 @@
       <c r="D4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the year production of oil in state of Alagoas?', 'SELECT year, oil_production FROM ANP WHERE lower(state) = ''alagoas''');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1125,8 +1189,12 @@
       <c r="D5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('fields are there in Paraná?', 'SELECT distinct field FROM ANP WHERE lower(state) = ''paraná''');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1139,8 +1207,12 @@
       <c r="D6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the production of oil in state of Ceará field?', 'SELECT oil_production, field FROM ANP WHERE lower(state) = ''ceará''');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1153,8 +1225,12 @@
       <c r="D7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the gas production in state of São Paulo basin?', 'SELECT gas_production, basin FROM ANP WHERE lower(state) = ''são paulo''');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1167,8 +1243,12 @@
       <c r="D8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month oil production of the operator Petrobras?', 'SELECT year, month, oil_production FROM ANP WHERE lower(operator) = ''petrobras''');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1181,8 +1261,12 @@
       <c r="D9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the year gas production field?', 'SELECT year, gas_production, field FROM ANP ');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1195,8 +1279,12 @@
       <c r="D10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the gas production month field?', 'SELECT gas_production, year, month, field FROM ANP ');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1209,8 +1297,12 @@
       <c r="D11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month gas production field?', 'SELECT year, month, gas_production, field FROM ANP ');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1223,8 +1315,12 @@
       <c r="D12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the field gas production month?', 'SELECT field, gas_production, year, month FROM ANP ');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1237,8 +1333,12 @@
       <c r="D13" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month petroleum production field in state of Rio de Janeiro?', 'SELECT year, month, field, oil_production FROM ANP WHERE lower(state) = ''rio de janeiro''');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1251,8 +1351,12 @@
       <c r="D14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the year petroleum production field by Rio de Janeiro?', 'SELECT year, field, oil_production FROM ANP WHERE lower(state) = ''rio de janeiro''');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1265,8 +1369,12 @@
       <c r="D15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month production of oil field in state of Rio de Janeiro and year 2015?', 'SELECT year, month, field, oil_production FROM ANP WHERE lower(state) = ''rio de janeiro'' and year = 2015');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1279,8 +1387,12 @@
       <c r="D16" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the year production of oil field state in the year of 2015?', 'SELECT year, oil_production, field, state FROM ANP WHERE year = 2015');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1293,8 +1405,12 @@
       <c r="D17" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the gas production field with production greater than 100 cubic meters?', 'SELECT gas_production, field FROM ANP WHERE gas_production &gt; 100');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1306,6 +1422,82 @@
       </c>
       <c r="D18" t="s">
         <v>58</v>
+      </c>
+      <c r="E18" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the gas production basin with production less than 1000 cubic meters?', 'SELECT gas_production, basin FROM ANP WHERE gas_production &lt; 1000');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('Which field produces the oil month?', 'SELECT field, oil_production, year, month FROM ANP ');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('Which basin has the year oil production?', 'SELECT basin, year, oil_production FROM ANP ');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('Which federated state has the gas production?', 'SELECT state, gas_production FROM ANP ');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" t="str">
+        <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('Which state of the federation has the gas production?', 'SELECT state, gas_production FROM ANP ');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Version Final Programming Project
</commit_message>
<xml_diff>
--- a/datasets/pfp.xlsx
+++ b/datasets/pfp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t>NLQ</t>
   </si>
@@ -33,48 +33,15 @@
     <t>GLAMORISE SQL</t>
   </si>
   <si>
-    <t>What was the production of oil in state of Rio de Janeiro?</t>
-  </si>
-  <si>
     <t>SELECT * FROM NLIDB_RESULT_SET</t>
   </si>
   <si>
-    <t>What was the average monthly production of oil in state of Rio de Janeiro?</t>
-  </si>
-  <si>
-    <t>What was the month production of oil in state of Rio de Janeiro?</t>
-  </si>
-  <si>
-    <t>What was the average yearly production of oil in state of Alagoas?</t>
-  </si>
-  <si>
-    <t>What was the year production of oil in state of Alagoas?</t>
-  </si>
-  <si>
     <t>How many fields are there in Paraná?</t>
   </si>
   <si>
     <t>fields are there in Paraná?</t>
   </si>
   <si>
-    <t>What was the maximum production of oil in state of Ceará per field?</t>
-  </si>
-  <si>
-    <t>What was the production of oil in state of Ceará field?</t>
-  </si>
-  <si>
-    <t>What was the minimum gas production in state of São Paulo per basin?</t>
-  </si>
-  <si>
-    <t>What was the gas production in state of São Paulo basin?</t>
-  </si>
-  <si>
-    <t>What was the average monthly oil production of the operator Petrobras?</t>
-  </si>
-  <si>
-    <t>What was the month oil production of the operator Petrobras?</t>
-  </si>
-  <si>
     <t>What was the mean yearly gas production per field?</t>
   </si>
   <si>
@@ -102,24 +69,12 @@
     <t xml:space="preserve">SELECT field, gas_production, year, month FROM ANP </t>
   </si>
   <si>
-    <t>What was the mean monthly petroleum production by field in state of Rio de Janeiro?</t>
-  </si>
-  <si>
-    <t>What was the month petroleum production field in state of Rio de Janeiro?</t>
-  </si>
-  <si>
     <t>What was the mean yearly petroleum production by field by Rio de Janeiro?</t>
   </si>
   <si>
     <t>What was the year petroleum production field by Rio de Janeiro?</t>
   </si>
   <si>
-    <t>What was the average monthly production of oil per field in state of Rio de Janeiro and year 2015?</t>
-  </si>
-  <si>
-    <t>What was the average yearly production of oil per field and state in the year of 2015?</t>
-  </si>
-  <si>
     <t>What was the mean gas production per field with production greater than 100 cubic meters?</t>
   </si>
   <si>
@@ -153,9 +108,6 @@
     <t>SELECT gas_production, basin FROM ANP WHERE lower(state) = 'são paulo'</t>
   </si>
   <si>
-    <t>SELECT year, month, oil_production FROM ANP WHERE lower(operator) = 'petrobras'</t>
-  </si>
-  <si>
     <t xml:space="preserve">SELECT year, gas_production, field FROM ANP </t>
   </si>
   <si>
@@ -177,12 +129,6 @@
     <t>SELECT year, oil_production, field, state FROM ANP WHERE year = 2015</t>
   </si>
   <si>
-    <t>What was the year production of oil field state in the year of 2015?</t>
-  </si>
-  <si>
-    <t>What was the month production of oil field in state of Rio de Janeiro and year 2015?</t>
-  </si>
-  <si>
     <t>What was the gas production field with production greater than 100 cubic meters?</t>
   </si>
   <si>
@@ -268,6 +214,66 @@
   </si>
   <si>
     <t>Which state of the federation has the gas production?</t>
+  </si>
+  <si>
+    <t>What was the production of oil in the state of Rio de Janeiro?</t>
+  </si>
+  <si>
+    <t>What was the average monthly production of oil in the state of Rio de Janeiro?</t>
+  </si>
+  <si>
+    <t>What was the month production of oil in the state of Rio de Janeiro?</t>
+  </si>
+  <si>
+    <t>What was the average yearly production of oil in the state of Alagoas?</t>
+  </si>
+  <si>
+    <t>What was the year production of oil in the state of Alagoas?</t>
+  </si>
+  <si>
+    <t>What was the maximum production of oil in the state of Ceará per field?</t>
+  </si>
+  <si>
+    <t>What was the production of oil in the state of Ceará field?</t>
+  </si>
+  <si>
+    <t>What was the minimum gas production in the state of São Paulo per basin?</t>
+  </si>
+  <si>
+    <t>What was the gas production in the state of São Paulo basin?</t>
+  </si>
+  <si>
+    <t>What was the mean monthly petroleum production by field in the state of Rio de Janeiro?</t>
+  </si>
+  <si>
+    <t>What was the month petroleum production field in the state of Rio de Janeiro?</t>
+  </si>
+  <si>
+    <t>What was the average monthly production of oil per field in the state of Rio de Janeiro and year 2015?</t>
+  </si>
+  <si>
+    <t>What was the average yearly production of oil per field and state in the year in 2015?</t>
+  </si>
+  <si>
+    <t>What was the year production of oil field state in the year in 2015?</t>
+  </si>
+  <si>
+    <t>What was the average monthly oil production by the operator Petrobrás?</t>
+  </si>
+  <si>
+    <t>SELECT year, month, oil_production, operator FROM ANP WHERE lower(operator) = 'petrobras'</t>
+  </si>
+  <si>
+    <t>What was the month production of oil field in the state of Rio de Janeiro year 2015?</t>
+  </si>
+  <si>
+    <t>What was the month oil production the operator Petrobrás?</t>
+  </si>
+  <si>
+    <t>select operator, avg(oil_production) as avg_oil_production from (select operator, sum(oil_production) as oil_production from nlidb_result_set group by operator, year, month) group by operator order by operator</t>
+  </si>
+  <si>
+    <t>select field, year, avg(oil_production) as avg_oil_production from (select field, year, sum(oil_production) as oil_production from nlidb_result_set group by field, year, year, month) group by field, year order by field, year</t>
   </si>
 </sst>
 </file>
@@ -1092,14 +1098,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:E22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="83.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="90.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="192.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="206.28515625" bestFit="1" customWidth="1"/>
@@ -1119,75 +1125,75 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
-        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the production of oil in state of Rio de Janeiro?', 'SELECT oil_production FROM ANP WHERE lower(state) = ''rio de janeiro''');</v>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the production of oil in the state of Rio de Janeiro?', 'SELECT oil_production FROM ANP WHERE lower(state) = ''rio de janeiro''');</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E3" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
-        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month production of oil in state of Rio de Janeiro?', 'SELECT year, month, oil_production FROM ANP WHERE lower(state) = ''rio de janeiro''');</v>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month production of oil in the state of Rio de Janeiro?', 'SELECT year, month, oil_production FROM ANP WHERE lower(state) = ''rio de janeiro''');</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E4" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
-        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the year production of oil in state of Alagoas?', 'SELECT year, oil_production FROM ANP WHERE lower(state) = ''alagoas''');</v>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the year production of oil in the state of Alagoas?', 'SELECT year, oil_production FROM ANP WHERE lower(state) = ''alagoas''');</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E5" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1196,70 +1202,70 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="E6" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
-        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the production of oil in state of Ceará field?', 'SELECT oil_production, field FROM ANP WHERE lower(state) = ''ceará''');</v>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the production of oil in the state of Ceará field?', 'SELECT oil_production, field FROM ANP WHERE lower(state) = ''ceará''');</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E7" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
-        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the gas production in state of São Paulo basin?', 'SELECT gas_production, basin FROM ANP WHERE lower(state) = ''são paulo''');</v>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the gas production in the state of São Paulo basin?', 'SELECT gas_production, basin FROM ANP WHERE lower(state) = ''são paulo''');</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="E8" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
-        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month oil production of the operator Petrobras?', 'SELECT year, month, oil_production FROM ANP WHERE lower(operator) = ''petrobras''');</v>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month oil production the operator Petrobrás?', 'SELECT year, month, oil_production, operator FROM ANP WHERE lower(operator) = ''petrobras''');</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="E9" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1268,16 +1274,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E10" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1286,16 +1292,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E11" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1304,16 +1310,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="E12" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1322,34 +1328,34 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E13" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
-        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month petroleum production field in state of Rio de Janeiro?', 'SELECT year, month, field, oil_production FROM ANP WHERE lower(state) = ''rio de janeiro''');</v>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month petroleum production field in the state of Rio de Janeiro?', 'SELECT year, month, field, oil_production FROM ANP WHERE lower(state) = ''rio de janeiro''');</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E14" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1358,52 +1364,52 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="E15" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
-        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month production of oil field in state of Rio de Janeiro and year 2015?', 'SELECT year, month, field, oil_production FROM ANP WHERE lower(state) = ''rio de janeiro'' and year = 2015');</v>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the month production of oil field in the state of Rio de Janeiro year 2015?', 'SELECT year, month, field, oil_production FROM ANP WHERE lower(state) = ''rio de janeiro'' and year = 2015');</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="E16" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
-        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the year production of oil field state in the year of 2015?', 'SELECT year, oil_production, field, state FROM ANP WHERE year = 2015');</v>
+        <v>INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('What was the year production of oil field state in the year in 2015?', 'SELECT year, oil_production, field, state FROM ANP WHERE year = 2015');</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E17" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1412,16 +1418,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E18" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1430,16 +1436,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E19" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1448,16 +1454,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="E20" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1466,16 +1472,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E21" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>
@@ -1484,16 +1490,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E22" t="str">
         <f>"INSERT INTO NLIDB_SQL_FROM_NLQ  VALUES('"&amp;Tabela1[[#This Row],[NLQ preproccessed by GLAMORISE]]&amp;"', '"&amp;SUBSTITUTE(Tabela1[[#This Row],[NLIDB SQL]],"'","''")&amp;"');"</f>

</xml_diff>